<commit_message>
added a lot of LCSC#s
</commit_message>
<xml_diff>
--- a/F405_pill_V1.1/F405_pill-pos.xlsx
+++ b/F405_pill_V1.1/F405_pill-pos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/kicad/F405_pill/F405_pill_V1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DF99994-2BDE-894E-BAED-5D0F363CAA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFE989C9-A338-FF4B-9AE9-495061611CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24780" yWindow="7500" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="20780" yWindow="5900" windowWidth="27640" windowHeight="16940"/>
   </bookViews>
   <sheets>
     <sheet name="F405_pill-pos" sheetId="1" r:id="rId1"/>

</xml_diff>